<commit_message>
download all permissions as template (need to optimize!)
</commit_message>
<xml_diff>
--- a/src/Framework.Configurator/Templates/Permissions.xlsx
+++ b/src/Framework.Configurator/Templates/Permissions.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15893E9F-3B76-4AB5-80BF-E3EE6408A50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F05C0F-670C-44AD-9E0E-31C6B4BBE6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82D28B7D-83E8-4640-AF53-5178E0B44E66}"/>
+    <workbookView xWindow="33555" yWindow="3030" windowWidth="23640" windowHeight="11280" xr2:uid="{82D28B7D-83E8-4640-AF53-5178E0B44E66}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Permissions" sheetId="1" r:id="rId1"/>
+    <sheet name="params" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Permissions!$A$1:$H$1</definedName>
+    <definedName name="PermissionsData">Permissions!$A$2:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Login</t>
   </si>
@@ -51,17 +53,53 @@
     <t>Remove</t>
   </si>
   <si>
-    <t>domain/login</t>
-  </si>
-  <si>
-    <t>Business Role Name</t>
+    <t>actions</t>
+  </si>
+  <si>
+    <t>{{item.Role}}</t>
+  </si>
+  <si>
+    <t>{{item.Login}}</t>
+  </si>
+  <si>
+    <t>{{item.ContextItems[0]}}</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>{{item.StartDate}}</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>{{item.EndDate}}</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>{{item.Comment}}</t>
+  </si>
+  <si>
+    <t>Permission id</t>
+  </si>
+  <si>
+    <t>{{item.Id}}</t>
+  </si>
+  <si>
+    <t>Context0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,24 +108,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,19 +139,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -124,10 +191,37 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4F004CF-B69D-48F6-9756-10DA2602B2FA}" name="PermissionsTable" displayName="PermissionsTable" ref="A1:H3" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:H3" xr:uid="{C4F004CF-B69D-48F6-9756-10DA2602B2FA}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{51796B4B-E325-41D9-B8A4-CE52ACDCC99E}" name="Action"/>
+    <tableColumn id="2" xr3:uid="{FAFFB297-6291-48D7-A059-1C462F76C177}" name="Login"/>
+    <tableColumn id="3" xr3:uid="{E658CC4A-341E-4B79-9C2B-F33F4F6C18DC}" name="Role"/>
+    <tableColumn id="7" xr3:uid="{96A0F4E3-0563-4A16-A08D-138D29BC6FA1}" name="Start date" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{61904F55-3291-459E-A322-F1FBE1C9A564}" name="End date" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{0F30E9D2-A5F1-42A5-B5B4-CFE15A144A7E}" name="Context0"/>
+    <tableColumn id="8" xr3:uid="{ACB6F9C7-2645-41DF-B71E-18623AFBD1E1}" name="Comment"/>
+    <tableColumn id="4" xr3:uid="{E62CCA6A-E054-4021-86B6-CD863F584755}" name="Permission id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C0EFDA5-B05C-4F81-A161-9B4E0A8FF675}" name="Actions" displayName="Actions" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3" xr:uid="{5C0EFDA5-B05C-4F81-A161-9B4E0A8FF675}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{14BA4B09-0F90-41E2-8B58-452995DC904F}" name="actions"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -165,7 +259,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -271,7 +365,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -413,7 +507,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,65 +515,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678B1921-A4B5-4353-8940-0FFC4450D337}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F628742B-7478-4A44-9096-97D89072EA04}">
+          <x14:formula1>
+            <xm:f>params!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Add/remove" xr:uid="{4499E44B-8011-440A-8A03-9CE0B125C175}">
+          <x14:formula1>
+            <xm:f>params!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0817189-4C9F-4FB6-820A-A8427D6D7091}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="12" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{678B1921-A4B5-4353-8940-0FFC4450D337}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>